<commit_message>
Updated code for displaying box and whisker plots for divergence and convergence analyses
</commit_message>
<xml_diff>
--- a/data/PRE_matrix__axonal_counts_per_neuron_per_parcel.xlsx
+++ b/data/PRE_matrix__axonal_counts_per_neuron_per_parcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drdiek/Sites/Projectomics/MATLAB/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC654436-2189-E44C-AE1A-874C3EA8219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F661D1-1FDE-0541-8A8B-6B962CE6B83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{561A34DF-2E63-3A44-BF1D-67C038364739}"/>
+    <workbookView xWindow="0" yWindow="2500" windowWidth="35840" windowHeight="21100" xr2:uid="{561A34DF-2E63-3A44-BF1D-67C038364739}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1113,10 +1113,17 @@
   <dimension ref="A1:ER94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>